<commit_message>
Excel file: catch incorrect column names and data type declaration
</commit_message>
<xml_diff>
--- a/inst/extdata/HrIssue/FRoc-Prostate.xlsx
+++ b/inst/extdata/HrIssue/FRoc-Prostate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkStation\临床试验-学习\诊断试验相关文献\MRMC-Rjafroc(markdown)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/HrIssue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8A6C05-4E0B-41B6-8843-9ECA91DEE0D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4B11E0-5BCD-3942-82CD-72D06396AC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="340" windowWidth="25360" windowHeight="15380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3440" yWindow="500" windowWidth="25360" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRUTH" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="12">
   <si>
     <t>CaseID</t>
   </si>
@@ -57,14 +57,17 @@
     <t>0,1</t>
   </si>
   <si>
-    <t>ROC</t>
-  </si>
-  <si>
     <t>FCTRL</t>
   </si>
   <si>
     <t>1,2,3,4</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TP_Rating</t>
+  </si>
+  <si>
+    <t>FROC</t>
   </si>
 </sst>
 </file>
@@ -75,7 +78,7 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -83,7 +86,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -91,13 +94,13 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -142,13 +145,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -487,19 +490,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="8.81640625" style="1"/>
+    <col min="1" max="3" width="8.83203125" style="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.31640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" style="1"/>
+    <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -530,36 +533,36 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -570,14 +573,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -588,14 +591,14 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -606,14 +609,14 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -624,14 +627,14 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -642,14 +645,14 @@
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -660,14 +663,14 @@
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -678,14 +681,14 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -696,14 +699,14 @@
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -714,14 +717,14 @@
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F12"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -732,14 +735,14 @@
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -750,13 +753,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -767,13 +770,13 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -784,13 +787,13 @@
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -801,13 +804,13 @@
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -818,13 +821,13 @@
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -835,13 +838,13 @@
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -852,13 +855,13 @@
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -869,13 +872,13 @@
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -886,13 +889,13 @@
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -903,13 +906,13 @@
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -920,13 +923,13 @@
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -937,13 +940,13 @@
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -954,13 +957,13 @@
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -971,13 +974,13 @@
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -988,13 +991,13 @@
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1005,13 +1008,13 @@
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1022,13 +1025,13 @@
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1039,13 +1042,13 @@
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -1056,13 +1059,13 @@
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -1073,13 +1076,13 @@
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1090,13 +1093,13 @@
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -1107,13 +1110,13 @@
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -1124,13 +1127,13 @@
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -1141,13 +1144,13 @@
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -1158,13 +1161,13 @@
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -1175,13 +1178,13 @@
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -1192,13 +1195,13 @@
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -1209,13 +1212,13 @@
         <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -1226,13 +1229,13 @@
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -1243,13 +1246,13 @@
         <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -1260,13 +1263,13 @@
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -1277,13 +1280,13 @@
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -1294,13 +1297,13 @@
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -1311,13 +1314,13 @@
         <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -1328,13 +1331,13 @@
         <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -1345,13 +1348,13 @@
         <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -1362,13 +1365,13 @@
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -1379,13 +1382,13 @@
         <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -1396,13 +1399,13 @@
         <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -1413,13 +1416,13 @@
         <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -1430,13 +1433,13 @@
         <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -1447,13 +1450,13 @@
         <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -1464,13 +1467,13 @@
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -1481,13 +1484,13 @@
         <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -1498,13 +1501,13 @@
         <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -1515,13 +1518,13 @@
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -1532,13 +1535,13 @@
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -1549,13 +1552,13 @@
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -1566,13 +1569,13 @@
         <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -1583,13 +1586,13 @@
         <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -1600,13 +1603,13 @@
         <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -1617,13 +1620,13 @@
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -1634,13 +1637,13 @@
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -1651,13 +1654,13 @@
         <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -1668,13 +1671,13 @@
         <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -1685,13 +1688,13 @@
         <v>1</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -1702,13 +1705,13 @@
         <v>1</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -1719,13 +1722,13 @@
         <v>1</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -1736,13 +1739,13 @@
         <v>1</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -1753,13 +1756,13 @@
         <v>1</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -1770,13 +1773,13 @@
         <v>1</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -1787,13 +1790,13 @@
         <v>1</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -1804,13 +1807,13 @@
         <v>1</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -1821,13 +1824,13 @@
         <v>1</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -1838,13 +1841,13 @@
         <v>1</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -1855,13 +1858,13 @@
         <v>1</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -1872,13 +1875,13 @@
         <v>1</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -1889,13 +1892,13 @@
         <v>1</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -1906,13 +1909,13 @@
         <v>1</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -1923,13 +1926,13 @@
         <v>1</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -1940,13 +1943,13 @@
         <v>1</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -1957,13 +1960,13 @@
         <v>1</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -1974,13 +1977,13 @@
         <v>1</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -1991,13 +1994,13 @@
         <v>1</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -2008,13 +2011,13 @@
         <v>1</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -2025,13 +2028,13 @@
         <v>1</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -2042,13 +2045,13 @@
         <v>1</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -2059,13 +2062,13 @@
         <v>1</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -2076,13 +2079,13 @@
         <v>1</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -2093,13 +2096,13 @@
         <v>1</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -2110,13 +2113,13 @@
         <v>1</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -2127,13 +2130,13 @@
         <v>1</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -2144,13 +2147,13 @@
         <v>1</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -2161,13 +2164,13 @@
         <v>1</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -2178,13 +2181,13 @@
         <v>1</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -2195,13 +2198,13 @@
         <v>1</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -2212,13 +2215,13 @@
         <v>1</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -2229,7 +2232,7 @@
         <v>1</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>7</v>
@@ -2252,18 +2255,15 @@
   <dimension ref="A1:D104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>1</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>1</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>2</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>2</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>2</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>2</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>2</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>2</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>2</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>2</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>2</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>2</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>2</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>2</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>2</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>2</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>2</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>2</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>2</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>3</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>3</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>3</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>3</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>3</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>3</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>3</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>3</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>3</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>3</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>3</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>3</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>3</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>3</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>3</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>3</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>3</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>3</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>3</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>3</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>3</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>3</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>3</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>3</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>3</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>3</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>3</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>3</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>3</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>3</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>3</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>3</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>3</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>3</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>3</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>3</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>3</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>3</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>3</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>3</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>3</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>4</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>4</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>4</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>4</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>4</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>4</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>4</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>4</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>1</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>1</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>2</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>2</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>2</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>2</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>2</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>2</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>2</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>2</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>2</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>2</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>2</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>2</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>3</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>3</v>
       </c>
@@ -3735,20 +3735,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="14" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3762,10 +3758,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3782,7 +3778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -3799,7 +3795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -3816,7 +3812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -3833,7 +3829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -3850,7 +3846,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -3867,7 +3863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -3884,7 +3880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -3901,7 +3897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -3918,7 +3914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -3935,7 +3931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -3952,7 +3948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -3969,7 +3965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -3986,7 +3982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -4003,7 +3999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>2</v>
       </c>
@@ -4020,7 +4016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -4037,7 +4033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>2</v>
       </c>
@@ -4054,7 +4050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>2</v>
       </c>
@@ -4071,7 +4067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -4088,7 +4084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>2</v>
       </c>
@@ -4105,7 +4101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>2</v>
       </c>
@@ -4122,7 +4118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>2</v>
       </c>
@@ -4139,7 +4135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -4156,7 +4152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>2</v>
       </c>
@@ -4173,7 +4169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>2</v>
       </c>
@@ -4190,7 +4186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>2</v>
       </c>
@@ -4207,7 +4203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>2</v>
       </c>
@@ -4224,7 +4220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>2</v>
       </c>
@@ -4241,7 +4237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>3</v>
       </c>
@@ -4258,7 +4254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>3</v>
       </c>
@@ -4275,7 +4271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>3</v>
       </c>
@@ -4292,7 +4288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>3</v>
       </c>
@@ -4309,7 +4305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>3</v>
       </c>
@@ -4326,7 +4322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>3</v>
       </c>
@@ -4343,7 +4339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>3</v>
       </c>
@@ -4360,7 +4356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>3</v>
       </c>
@@ -4377,7 +4373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>3</v>
       </c>
@@ -4394,7 +4390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>3</v>
       </c>
@@ -4411,7 +4407,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>3</v>
       </c>
@@ -4428,7 +4424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>3</v>
       </c>
@@ -4445,7 +4441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>3</v>
       </c>
@@ -4462,7 +4458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>3</v>
       </c>
@@ -4479,7 +4475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>3</v>
       </c>
@@ -4496,7 +4492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>3</v>
       </c>
@@ -4513,7 +4509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>3</v>
       </c>
@@ -4530,7 +4526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>3</v>
       </c>
@@ -4547,7 +4543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>3</v>
       </c>
@@ -4564,7 +4560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>3</v>
       </c>
@@ -4581,7 +4577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>3</v>
       </c>
@@ -4598,7 +4594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>3</v>
       </c>
@@ -4615,7 +4611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>3</v>
       </c>
@@ -4632,7 +4628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>3</v>
       </c>
@@ -4649,7 +4645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>3</v>
       </c>
@@ -4666,7 +4662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>3</v>
       </c>
@@ -4683,7 +4679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>3</v>
       </c>
@@ -4700,7 +4696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>3</v>
       </c>
@@ -4717,7 +4713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>3</v>
       </c>
@@ -4734,7 +4730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>3</v>
       </c>
@@ -4751,7 +4747,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>4</v>
       </c>
@@ -4768,7 +4764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>4</v>
       </c>
@@ -4785,7 +4781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>4</v>
       </c>
@@ -4802,7 +4798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>4</v>
       </c>
@@ -4819,7 +4815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>4</v>
       </c>
@@ -4836,7 +4832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>4</v>
       </c>
@@ -4853,7 +4849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>4</v>
       </c>
@@ -4870,7 +4866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>4</v>
       </c>
@@ -4887,7 +4883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>4</v>
       </c>
@@ -4904,7 +4900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>4</v>
       </c>
@@ -4921,7 +4917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>4</v>
       </c>
@@ -4938,7 +4934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>4</v>
       </c>
@@ -4955,7 +4951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>4</v>
       </c>
@@ -4972,7 +4968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>4</v>
       </c>
@@ -4989,7 +4985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>1</v>
       </c>
@@ -5006,7 +5002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>2</v>
       </c>
@@ -5023,7 +5019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>2</v>
       </c>
@@ -5040,7 +5036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>2</v>
       </c>
@@ -5057,7 +5053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>2</v>
       </c>
@@ -5074,7 +5070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>2</v>
       </c>
@@ -5091,7 +5087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>2</v>
       </c>
@@ -5108,7 +5104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>2</v>
       </c>
@@ -5125,7 +5121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>2</v>
       </c>
@@ -5142,7 +5138,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>2</v>
       </c>
@@ -5159,7 +5155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>2</v>
       </c>
@@ -5176,7 +5172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>2</v>
       </c>
@@ -5193,7 +5189,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>3</v>
       </c>
@@ -5210,7 +5206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>3</v>
       </c>
@@ -5227,7 +5223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>3</v>
       </c>
@@ -5244,7 +5240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>4</v>
       </c>

</xml_diff>